<commit_message>
Schema changed! Fixed #198
Added Decision Kinds
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/ColorsSettings.xlsx
+++ b/DatabaseUpdate/ExcelFiles/ColorsSettings.xlsx
@@ -34,37 +34,37 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>Pale Green</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|inProgressCommission|</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#98FB98</x:t>
+    <x:t>|CommissionDecisionNegative|</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Отрицательное решение</x:t>
+  </x:si>
+  <x:si>
+    <x:t>#FF8375</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
-    <x:t>Tomato</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|deniedCommission|</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#f45b5b</x:t>
+    <x:t>|CommissionDecisionNeutral|</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Нейтральное решение</x:t>
+  </x:si>
+  <x:si>
+    <x:t>#FFF293</x:t>
   </x:si>
   <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
-    <x:t>LemonChiffon</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|completedCommission|</x:t>
-  </x:si>
-  <x:si>
-    <x:t>#f2f2b0</x:t>
+    <x:t>|CommissionDecisionPositive|</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Положительное решение</x:t>
+  </x:si>
+  <x:si>
+    <x:t>#4CFF76</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -442,13 +442,13 @@
       <x:c r="A2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="B2" s="0" t="s"/>
+      <x:c r="C2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s"/>
       <x:c r="E2" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
@@ -457,13 +457,13 @@
       <x:c r="A3" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+      <x:c r="B3" s="0" t="s"/>
+      <x:c r="C3" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
+      <x:c r="D3" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s"/>
       <x:c r="E3" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -472,13 +472,13 @@
       <x:c r="A4" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="B4" s="0" t="s"/>
+      <x:c r="C4" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s"/>
       <x:c r="E4" s="0" t="s">
         <x:v>16</x:v>
       </x:c>

</xml_diff>